<commit_message>
Novas alterações do Renato
Adição de gráficos e algumas outras modificações
</commit_message>
<xml_diff>
--- a/data/universalizacao_pre_escola_linha_15-20.xlsx
+++ b/data/universalizacao_pre_escola_linha_15-20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yajeon\Documents\GitHub\app_tcm_ideb\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app_tcm_ideb-main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87ADC9E-1F2D-4166-8854-480113B402DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EAE0E1-0029-4D60-A181-297B2CA097C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="825" windowWidth="9750" windowHeight="7905" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LINHA evol indic mun (15-20)" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>[ODS.04.02] Taxa de Universalização da Educação Infantil (somente pré-escola) (%)</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Populacao</t>
+  </si>
+  <si>
+    <t>Ano</t>
   </si>
 </sst>
 </file>
@@ -523,20 +526,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="12" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="10.42578125" customWidth="1"/>
     <col min="17" max="17" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -756,14 +759,19 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>10</v>
@@ -771,7 +779,6 @@
       <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3"/>
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Mudanças propostas por Sofia e Marian
Arrumando detalhes de indentação

Tornando o modo escuro um pouco mais claro para melhor contraste do fundo com os gráficos

Alterando todos os textos (exceto links) para branco

Substituindo os links da tela principal por links mais relevantes enviados pela Marian

Trocando a imagem da tela inicial pelo logo do Observatório

Deixando os gráficos com cores mais chamativas

Alterando o mapa de universalização para um gráfico de linhas RME
</commit_message>
<xml_diff>
--- a/data/universalizacao_pre_escola_linha_15-20.xlsx
+++ b/data/universalizacao_pre_escola_linha_15-20.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app_tcm_ideb-main\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yajeon\Documents\GitHub\app_tcm_ideb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EAE0E1-0029-4D60-A181-297B2CA097C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87ECFDA-A13D-4B3A-867F-505C9B993809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LINHA evol indic mun (15-20)" sheetId="7" r:id="rId1"/>
     <sheet name="LINHA evol. var mun (15-20)" sheetId="21" r:id="rId2"/>
+    <sheet name="LINHA evol. matr. RME (15-20)" sheetId="22" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>[ODS.04.02] Taxa de Universalização da Educação Infantil (somente pré-escola) (%)</t>
   </si>
@@ -69,6 +70,24 @@
   </si>
   <si>
     <t>Ano</t>
+  </si>
+  <si>
+    <t>Matrículas na Pré-Escola da Rede Municipal de Ensino</t>
+  </si>
+  <si>
+    <t>&lt;- deixar esse nome no gráfico</t>
+  </si>
+  <si>
+    <t>Variável</t>
+  </si>
+  <si>
+    <t>Demanda atendida de vagas em pré-escolas da rede municipal de ensino (%)</t>
+  </si>
+  <si>
+    <t>Matrículas na Pré-Escola da rede municipal de ensino</t>
+  </si>
+  <si>
+    <t>Fonte: Indicador "Demanda atendida de vagas de pré-escola da RME".</t>
   </si>
 </sst>
 </file>
@@ -107,7 +126,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,7 +176,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -182,6 +207,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -758,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984308DC-C5BE-4D60-8339-0A4A59779BA9}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1015,4 +1049,275 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D802D8E-984E-46AF-9D17-507A6BF6BB13}">
+  <dimension ref="A1:Q12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2" s="13">
+        <v>288403</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+    </row>
+    <row r="3" spans="1:17" ht="30.75" thickBot="1">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3" s="13">
+        <v>185134</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="12">
+        <v>2010</v>
+      </c>
+      <c r="H3" s="12">
+        <v>2011</v>
+      </c>
+      <c r="I3" s="12">
+        <v>2012</v>
+      </c>
+      <c r="J3" s="12">
+        <v>2013</v>
+      </c>
+      <c r="K3" s="12">
+        <v>2014</v>
+      </c>
+      <c r="L3" s="12">
+        <v>2015</v>
+      </c>
+      <c r="M3" s="12">
+        <v>2016</v>
+      </c>
+      <c r="N3" s="12">
+        <v>2017</v>
+      </c>
+      <c r="O3" s="12">
+        <v>2018</v>
+      </c>
+      <c r="P3" s="12">
+        <v>2019</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="165.75" thickBot="1">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4" s="13">
+        <v>183257</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="13">
+        <v>288403</v>
+      </c>
+      <c r="H4" s="13">
+        <v>185134</v>
+      </c>
+      <c r="I4" s="13">
+        <v>183257</v>
+      </c>
+      <c r="J4" s="13">
+        <v>200369</v>
+      </c>
+      <c r="K4" s="13">
+        <v>202294</v>
+      </c>
+      <c r="L4" s="13">
+        <v>204513</v>
+      </c>
+      <c r="M4" s="13">
+        <v>215049</v>
+      </c>
+      <c r="N4" s="13">
+        <v>219094</v>
+      </c>
+      <c r="O4" s="13">
+        <v>218029</v>
+      </c>
+      <c r="P4" s="13">
+        <v>223280</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>235662</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="13">
+        <v>200369</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="13">
+        <v>202294</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A7" s="10">
+        <v>2015</v>
+      </c>
+      <c r="B7" s="13">
+        <v>204513</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8" s="13">
+        <v>215049</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="13">
+        <v>219094</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10" s="13">
+        <v>218029</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11" s="13">
+        <v>223280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12" s="13">
+        <v>235662</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>